<commit_message>
Update Motivation, Team, Passive
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Resources/Documents/OneAbility/OneAbilityInfo.xlsx
+++ b/Assets/Scripts/1.Abilities/Resources/Documents/OneAbility/OneAbilityInfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Resources\Documents\OneAbility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Resources\Documents\OneAbility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3C4221-B840-41F5-AB39-A4187A412846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78078791-E661-48D0-9B70-BF28EB99D397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8910" yWindow="5410" windowWidth="28800" windowHeight="15460" activeTab="3" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
+    <workbookView xWindow="3495" yWindow="3495" windowWidth="28800" windowHeight="15345" activeTab="4" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
   </bookViews>
   <sheets>
     <sheet name="AreaAbility" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="15">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -471,16 +471,16 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="6.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,98 +508,93 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.3">
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.3">
       <c r="Q24" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="H2:J2"/>
@@ -612,6 +607,11 @@
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -626,16 +626,16 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -663,42 +663,42 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -728,9 +728,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -758,83 +758,89 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
     <mergeCell ref="H13:J13"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
@@ -845,12 +851,6 @@
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -861,13 +861,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C104C1DD-5DC9-4B96-B8AF-A07D98126122}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -892,57 +892,57 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -969,22 +969,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC57950A-9E23-4278-A211-D37973D388E6}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.33203125" customWidth="1"/>
+    <col min="4" max="6" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -995,92 +994,89 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1095,7 +1091,7 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
@@ -1105,7 +1101,7 @@
     <col min="6" max="8" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1136,52 +1132,52 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="25" spans="10:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>13</v>
       </c>
@@ -1212,15 +1208,15 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1248,32 +1244,32 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>

</xml_diff>